<commit_message>
Estas son las notas finales, mañana empiezo la mocha, digo, a publicar
</commit_message>
<xml_diff>
--- a/OYM/_DocumentosComunes/Algoritmo.xlsx
+++ b/OYM/_DocumentosComunes/Algoritmo.xlsx
@@ -837,11 +837,11 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H3:H39"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2518,6 +2518,11 @@
         <v>70</v>
       </c>
     </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B40">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:O1">
     <filterColumn colId="1" showButton="0"/>

</xml_diff>